<commit_message>
v 043 - feb 25
</commit_message>
<xml_diff>
--- a/docs/v043/StructureDefinition-BundleCo.xlsx
+++ b/docs/v043/StructureDefinition-BundleCo.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-10T08:50:18-03:00</t>
+    <t>2025-02-21T13:43:19-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -625,7 +625,7 @@
 * Results from operations might involve resources that are not identified.</t>
   </si>
   <si>
-    <t>fullUrl might not be [unique in the context of a resource](bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
+    <t>fullUrl might not be [unique in the context of a resource](http://hl7.org/fhir/R4/bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
 Note that the fullUrl is not the same as the canonical URL - it's an absolute url for an endpoint serving the resource (these will happen to have the same value on the canonical server for the resource with the canonical URL).</t>
   </si>
   <si>
@@ -8259,7 +8259,7 @@
         <v>87</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>77</v>
@@ -11885,7 +11885,7 @@
         <v>87</v>
       </c>
       <c r="H87" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I87" t="s" s="2">
         <v>77</v>
@@ -15509,7 +15509,7 @@
         <v>87</v>
       </c>
       <c r="H119" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I119" t="s" s="2">
         <v>77</v>
@@ -19135,7 +19135,7 @@
         <v>87</v>
       </c>
       <c r="H151" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I151" t="s" s="2">
         <v>77</v>
@@ -22759,7 +22759,7 @@
         <v>87</v>
       </c>
       <c r="H183" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I183" t="s" s="2">
         <v>77</v>
@@ -26385,7 +26385,7 @@
         <v>87</v>
       </c>
       <c r="H215" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I215" t="s" s="2">
         <v>77</v>
@@ -30011,7 +30011,7 @@
         <v>87</v>
       </c>
       <c r="H247" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I247" t="s" s="2">
         <v>77</v>

</xml_diff>